<commit_message>
Refine API specs and other misc changes
</commit_message>
<xml_diff>
--- a/api/api-specs.xlsx
+++ b/api/api-specs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t xml:space="preserve">Endpoints</t>
   </si>
@@ -67,16 +67,61 @@
     <t xml:space="preserve">{data:{rooms:[]}}</t>
   </si>
   <si>
+    <t xml:space="preserve">/api/rooms/:id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data:{room:{}}}</t>
+  </si>
+  <si>
     <t xml:space="preserve">/api/rooms/create</t>
   </si>
   <si>
-    <t xml:space="preserve">{data:{room}</t>
+    <t xml:space="preserve">{number,baseRent}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The newly created Room</t>
   </si>
   <si>
     <t xml:space="preserve">/api/tenants</t>
   </si>
   <si>
+    <t xml:space="preserve">{data:{tenants:[]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/tenants/:id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data:{tenant:{}}}</t>
+  </si>
+  <si>
     <t xml:space="preserve">/api/tenants/create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{name,phoneNumber,aadharCard,room}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The newly created Tenant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/transactions/?room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data:{transactions:[]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/transactions/:id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data:{transaction:{}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/tenants/create/?roomNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{room,balance,transfer,remarks}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The newly created Transaction</t>
   </si>
 </sst>
 </file>
@@ -191,16 +236,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI32"/>
+  <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="89.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="11.52"/>
@@ -577,7 +622,7 @@
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="0"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -611,10 +656,18 @@
       <c r="AI10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="0"/>
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -648,13 +701,9 @@
       <c r="AI11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -690,11 +739,11 @@
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -730,9 +779,13 @@
       <c r="AI13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -767,10 +820,18 @@
       <c r="AI14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -841,10 +902,14 @@
       <c r="AI16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="0"/>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -878,9 +943,13 @@
       <c r="AI17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -915,10 +984,18 @@
       <c r="AI18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1432,6 +1509,80 @@
       <c r="AH32" s="2"/>
       <c r="AI32" s="2"/>
     </row>
+    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2"/>
+      <c r="AF33" s="2"/>
+      <c r="AG33" s="2"/>
+      <c r="AH33" s="2"/>
+      <c r="AI33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
+      <c r="AF34" s="2"/>
+      <c r="AG34" s="2"/>
+      <c r="AH34" s="2"/>
+      <c r="AI34" s="2"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
refine api specs and readme
</commit_message>
<xml_diff>
--- a/api/api-specs.xlsx
+++ b/api/api-specs.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t xml:space="preserve">Endpoints</t>
   </si>
   <si>
-    <t xml:space="preserve">Input inside body</t>
+    <t xml:space="preserve">Method/Input inside body</t>
   </si>
   <si>
     <t xml:space="preserve">Retrun type</t>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">/</t>
   </si>
   <si>
+    <t xml:space="preserve">get</t>
+  </si>
+  <si>
     <t xml:space="preserve">html</t>
   </si>
   <si>
@@ -46,7 +49,7 @@
     <t xml:space="preserve">/api</t>
   </si>
   <si>
-    <t xml:space="preserve">{data:”/api accessible”}</t>
+    <t xml:space="preserve">{data:{message:”/api accessible”}}</t>
   </si>
   <si>
     <t xml:space="preserve">nothing in particular makes sense here</t>
@@ -55,6 +58,9 @@
     <t xml:space="preserve">/api/login</t>
   </si>
   <si>
+    <t xml:space="preserve">post/{username,password}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{data:{token}}</t>
   </si>
   <si>
@@ -73,10 +79,19 @@
     <t xml:space="preserve">{data:{room:{}}}</t>
   </si>
   <si>
+    <t xml:space="preserve">delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data:{message:”success”}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note the special delete method</t>
+  </si>
+  <si>
     <t xml:space="preserve">/api/rooms/create</t>
   </si>
   <si>
-    <t xml:space="preserve">{number,baseRent}</t>
+    <t xml:space="preserve">post/{number,baseRent}</t>
   </si>
   <si>
     <t xml:space="preserve">The newly created Room</t>
@@ -118,7 +133,7 @@
     <t xml:space="preserve">/api/tenants/create/?roomNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">{room,balance,transfer,remarks}</t>
+    <t xml:space="preserve">post/{room,balance,transfer,remarks}</t>
   </si>
   <si>
     <t xml:space="preserve">The newly created Transaction</t>
@@ -236,10 +251,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI34"/>
+  <dimension ref="A1:AI36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -337,12 +352,14 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -415,14 +432,16 @@
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -495,14 +514,16 @@
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -575,11 +596,13 @@
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -616,11 +639,13 @@
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -660,13 +685,13 @@
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -701,10 +726,18 @@
       <c r="AI11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -738,13 +771,9 @@
       <c r="AI12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -780,11 +809,11 @@
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -821,17 +850,13 @@
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -865,9 +890,15 @@
       <c r="AI15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -903,13 +934,17 @@
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -943,13 +978,9 @@
       <c r="AI17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -985,17 +1016,15 @@
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1029,9 +1058,15 @@
       <c r="AI19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1066,10 +1101,18 @@
       <c r="AI20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1583,6 +1626,80 @@
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
     </row>
+    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+      <c r="AA35" s="2"/>
+      <c r="AB35" s="2"/>
+      <c r="AC35" s="2"/>
+      <c r="AD35" s="2"/>
+      <c r="AE35" s="2"/>
+      <c r="AF35" s="2"/>
+      <c r="AG35" s="2"/>
+      <c r="AH35" s="2"/>
+      <c r="AI35" s="2"/>
+    </row>
+    <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="2"/>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
+      <c r="AF36" s="2"/>
+      <c r="AG36" s="2"/>
+      <c r="AH36" s="2"/>
+      <c r="AI36" s="2"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
implement user signup and delete
</commit_message>
<xml_diff>
--- a/api/api-specs.xlsx
+++ b/api/api-specs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t xml:space="preserve">Endpoints</t>
   </si>
@@ -67,6 +67,21 @@
     <t xml:space="preserve">token should be a jwt token</t>
   </si>
   <si>
+    <t xml:space="preserve">/api/signup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post/{username,password,email}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/signout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data:{message:”success}}</t>
+  </si>
+  <si>
     <t xml:space="preserve">/api/rooms</t>
   </si>
   <si>
@@ -77,9 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">{data:{room:{}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delete</t>
   </si>
   <si>
     <t xml:space="preserve">{data:{message:”success”}}</t>
@@ -251,10 +263,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI36"/>
+  <dimension ref="A1:AI38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -558,9 +570,15 @@
       <c r="AI7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -596,13 +614,13 @@
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -638,15 +656,9 @@
       <c r="AI9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -682,17 +694,15 @@
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -730,14 +740,12 @@
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -771,10 +779,18 @@
       <c r="AI12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -809,13 +825,17 @@
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -849,13 +869,9 @@
       <c r="AI14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -891,13 +907,11 @@
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -934,17 +948,13 @@
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -978,9 +988,15 @@
       <c r="AI17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1016,15 +1032,17 @@
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1058,15 +1076,9 @@
       <c r="AI19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1104,15 +1116,13 @@
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1146,9 +1156,15 @@
       <c r="AI21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1183,10 +1199,18 @@
       <c r="AI22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1700,6 +1724,80 @@
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
     </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+      <c r="AA37" s="2"/>
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="2"/>
+      <c r="AF37" s="2"/>
+      <c r="AG37" s="2"/>
+      <c r="AH37" s="2"/>
+      <c r="AI37" s="2"/>
+    </row>
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
+      <c r="AA38" s="2"/>
+      <c r="AB38" s="2"/>
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="2"/>
+      <c r="AF38" s="2"/>
+      <c r="AG38" s="2"/>
+      <c r="AH38" s="2"/>
+      <c r="AI38" s="2"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>